<commit_message>
Commit changes to the Add Trails JSP.  Also commit addition of my video and time log.
</commit_message>
<xml_diff>
--- a/Enterprise_Java_Time_Tracking.xlsx
+++ b/Enterprise_Java_Time_Tracking.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
   <si>
     <t>Monday</t>
   </si>
@@ -181,6 +181,141 @@
   </si>
   <si>
     <t>3.5 hrs - Perform code reviews for Sasha and Kyle.  Looked at how bootstrap works and how to add it to my .jsp's.</t>
+  </si>
+  <si>
+    <t>2 hrs - continued setup of AWS</t>
+  </si>
+  <si>
+    <t>4 hrs - Continued working through bugs for the setup of AWS</t>
+  </si>
+  <si>
+    <t>3 hrs - Continued trying to resolve issue with a 500 exception that won't allow my application to search the database.</t>
+  </si>
+  <si>
+    <t>3 hrs - Began putting together the slide show for my Professional presentation.  Began creating the Generic Dao for my project.
+3 hrs - Continued trying to resolve issue with a 500 exception that won't allow my application to search the database.</t>
+  </si>
+  <si>
+    <t>2.5 hrs -  Continued trying to resolve issue with a 500 exception that won't allow my application to search the database.</t>
+  </si>
+  <si>
+    <t>2.5 hrs - Resolved the issue with the 500 error and continued pushing my project to AWS</t>
+  </si>
+  <si>
+    <t>2.5 hrs - Continued watching the Week 8 video's and began walking through Activity 2 and Activity 3.</t>
+  </si>
+  <si>
+    <t>2.5 - Continued working on my Agile presentation.</t>
+  </si>
+  <si>
+    <t>2 hrs - began working on my Agile presentation.</t>
+  </si>
+  <si>
+    <t>2.5 hrs - Continued working on my Agile presentation and began watching the Week 8 video's and began walking through Activity 1.</t>
+  </si>
+  <si>
+    <t>4 hrs - Gave my Agile presentation and continued working on the Week 8 Activities</t>
+  </si>
+  <si>
+    <t>2.5 hrs - Continued working on Activity 3 to get the SOAP API test working.</t>
+  </si>
+  <si>
+    <t>2 hrs - Completed the Week 8 SOAP API assignment and turned it in.</t>
+  </si>
+  <si>
+    <t>1.5 hrs - Continued working on my indie project</t>
+  </si>
+  <si>
+    <t>3 hrs - Continued working on my indie project.  Worked on getting .jsp's created for Check point 3</t>
+  </si>
+  <si>
+    <t>3 - Met for the first time with the team and decided to create an Event Service.  Began talking through what types of end points we'd like this service to have.</t>
+  </si>
+  <si>
+    <t>2 hrs - worked through the week 9 Demo/Exercise to get an idea of how Restful services work</t>
+  </si>
+  <si>
+    <t>2 hrs - continued working  through the week 9 Demo/Exercise to get an idea of how Restful services work</t>
+  </si>
+  <si>
+    <t>2 hrs - began adding the Event Service to the team project.  Created the Search end point and tried testing it</t>
+  </si>
+  <si>
+    <t>3 hrs - continued testing the search endpoint and added the Add and Delete endpoints.</t>
+  </si>
+  <si>
+    <t>3 hrs - finished the week 9 Restful service exercise and continued testing the Event service team project</t>
+  </si>
+  <si>
+    <t>3.5 hrs - Worked with Steve and Kia to get the Event Services working correctly with the Dao and .jsp's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 hrs - continued working on the Event Service to get the search working correctly and get the add and delete working successfully  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 hrs - continued working on the Event Service to get the search working correctly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 hrs - continued working on the Event Service to add and delete working successfully  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 hrs - met with Steve and Kia to clean up our code and get everything pushed to github
+3 hrs - continued working on the Event Service to get the search working correctly so that it only brings back rows for a specific date range  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 hrs - continued working on the Event Service to get the search working correctly so that it only brings back rows for a specific date range  </t>
+  </si>
+  <si>
+    <t>4 hrs - finished cleaning up the Event Service code and making sure all of the output looks correct and everything is working  correctly</t>
+  </si>
+  <si>
+    <t>2 hrs - Give Event Service presentation in class and listen to other presentations</t>
+  </si>
+  <si>
+    <t>2 hrs - Filled out Team project survey.  Worked on getting back up to speed on indie project</t>
+  </si>
+  <si>
+    <t>2.5 hrs - Worked on creating the Hiking Trails jsp</t>
+  </si>
+  <si>
+    <t>2.5 hrs - worked on the week 13 exercise</t>
+  </si>
+  <si>
+    <t>1.5 hrs - worked on the week 13 exercise
+3 hrs - worked on getting user authentication working for my indie project</t>
+  </si>
+  <si>
+    <t>2 hrs - continued working on getting authentication working for the indie project</t>
+  </si>
+  <si>
+    <t>3 hrs - Worked on trying to get tabs to work for the menu options of my indie project</t>
+  </si>
+  <si>
+    <t>3.5 hrs - Worked on getting the Add Trails .jsp and the Login .jsp formatted correctly and working</t>
+  </si>
+  <si>
+    <t>4 hrs - Worked on getting my Search page working correctly.</t>
+  </si>
+  <si>
+    <t>3 hrs - Worked on getting my Search page working correctly.</t>
+  </si>
+  <si>
+    <t>3 hrs - Worked on getting the Search table scrolling to work correctly</t>
+  </si>
+  <si>
+    <t>3 hrs - Worked on the look and feel of the page correct</t>
+  </si>
+  <si>
+    <t>3 hrs - Worked on making sure all of the pages have the same look and feel</t>
+  </si>
+  <si>
+    <t>5 hrs - Worked on getting all of the documentation added and Java Doc created.  Created the required video.  Worked on trying to fix an issue that popped up with the Add Trail page.</t>
+  </si>
+  <si>
+    <t>3 hrs - Worked on trying to get the project to work correctly in AWS</t>
+  </si>
+  <si>
+    <t>4 hrs - Worked on getting my search results page formatted correctly with scrolling detail rows and a fixed header row.</t>
   </si>
 </sst>
 </file>
@@ -537,7 +672,9 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,116 +840,227 @@
       <c r="F7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">

</xml_diff>